<commit_message>
mark attendance for step school is ready now
</commit_message>
<xml_diff>
--- a/stud_data/FY1.xlsx
+++ b/stud_data/FY1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,36 @@
           <t>01-04-2025 Time</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>05-04-2025 Status</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>05-04-2025 Time</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>06-04-2025 Status</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>06-04-2025 Time</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>07-04-2025 Status</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>07-04-2025 Time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -532,7 +562,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -602,6 +632,28 @@
       <c r="Q2" t="inlineStr">
         <is>
           <t>09:35:20 AM</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>09:42:38 AM</t>
         </is>
       </c>
     </row>
@@ -617,7 +669,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -687,6 +739,28 @@
       <c r="Q3" t="inlineStr">
         <is>
           <t>09:35:31 AM</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>09:42:52 AM</t>
         </is>
       </c>
     </row>
@@ -702,7 +776,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -772,6 +846,28 @@
       <c r="Q4" t="inlineStr">
         <is>
           <t>09:35:35 AM</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>09:42:56 AM</t>
         </is>
       </c>
     </row>
@@ -787,7 +883,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -857,6 +953,28 @@
       <c r="Q5" t="inlineStr">
         <is>
           <t>09:35:39 AM</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>09:43:00 AM</t>
         </is>
       </c>
     </row>
@@ -872,7 +990,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -942,6 +1060,28 @@
       <c r="Q6" t="inlineStr">
         <is>
           <t>09:35:48 AM</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>09:43:10 AM</t>
         </is>
       </c>
     </row>
@@ -1029,6 +1169,28 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1042,7 +1204,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1112,6 +1274,28 @@
       <c r="Q8" t="inlineStr">
         <is>
           <t>09:35:57 AM</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>09:43:22 AM</t>
         </is>
       </c>
     </row>
@@ -1199,6 +1383,28 @@
           <t>09:36:02 AM</t>
         </is>
       </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1212,7 +1418,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1282,6 +1488,28 @@
       <c r="Q10" t="inlineStr">
         <is>
           <t>09:36:05 AM</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W10" t="inlineStr">
+        <is>
+          <t>09:43:26 AM</t>
         </is>
       </c>
     </row>
@@ -1369,6 +1597,28 @@
           <t>09:36:08 AM</t>
         </is>
       </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W11" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1454,6 +1704,28 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W12" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1539,6 +1811,28 @@
           <t>09:36:16 AM</t>
         </is>
       </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1552,7 +1846,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1622,6 +1916,28 @@
       <c r="Q14" t="inlineStr">
         <is>
           <t>09:36:23 AM</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W14" t="inlineStr">
+        <is>
+          <t>09:43:52 AM</t>
         </is>
       </c>
     </row>
@@ -1637,7 +1953,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1707,6 +2023,28 @@
       <c r="Q15" t="inlineStr">
         <is>
           <t>09:36:26 AM</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>09:43:55 AM</t>
         </is>
       </c>
     </row>
@@ -1722,7 +2060,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1792,6 +2130,28 @@
       <c r="Q16" t="inlineStr">
         <is>
           <t>09:36:32 AM</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="W16" t="inlineStr">
+        <is>
+          <t>09:43:59 AM</t>
         </is>
       </c>
     </row>
@@ -1879,6 +2239,28 @@
           <t>09:36:35 AM</t>
         </is>
       </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1964,6 +2346,28 @@
           <t>09:36:40 AM</t>
         </is>
       </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2049,6 +2453,28 @@
           <t>09:36:45 AM</t>
         </is>
       </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2134,6 +2560,28 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2219,6 +2667,28 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2304,6 +2774,28 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2389,6 +2881,28 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2470,6 +2984,28 @@
         </is>
       </c>
       <c r="Q24" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="W24" t="inlineStr">
         <is>
           <t>00:00:00</t>
         </is>

</xml_diff>

<commit_message>
here is the project with main file only
</commit_message>
<xml_diff>
--- a/stud_data/FY1.xlsx
+++ b/stud_data/FY1.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,6 +459,36 @@
           <t>07-04-2025 Time</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>05-04-2025 Status</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>05-04-2025 Time</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>09-04-2025 Status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>09-04-2025 Time</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>10-04-2025 Status</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>10-04-2025 Time</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -484,6 +514,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -509,6 +565,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -534,6 +616,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -559,6 +667,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -584,6 +718,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -609,6 +769,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -634,6 +820,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -659,6 +871,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -684,6 +922,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -709,6 +973,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -734,6 +1024,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -759,6 +1075,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -784,6 +1126,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -809,6 +1177,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -834,6 +1228,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -859,6 +1279,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -872,14 +1318,40 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
+        <is>
+          <t>08:46:24 AM</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>00:00:00</t>
         </is>
@@ -897,14 +1369,40 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>P</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
+        <is>
+          <t>08:46:03 AM</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>00:00:00</t>
         </is>
@@ -934,6 +1432,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -959,6 +1483,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -984,6 +1534,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1009,6 +1585,32 @@
           <t>00:00:00</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1030,6 +1632,32 @@
         </is>
       </c>
       <c r="E24" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Off</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>00:00:00</t>
         </is>

</xml_diff>